<commit_message>
Made graphs for summary slides
</commit_message>
<xml_diff>
--- a/LacTissueT1LBound10.xlsx
+++ b/LacTissueT1LBound10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12621C0D-0957-4C99-858A-A43BB48A8D59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC85DE3-5188-47A9-B7F1-15ECE56D2345}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D1CEB774-CC90-42A4-8F95-9A6C97CFD06A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
   <si>
     <t>Normal</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>FlowL</t>
+  </si>
+  <si>
+    <t>kpl</t>
+  </si>
+  <si>
+    <t>kLEfflux</t>
   </si>
 </sst>
 </file>
@@ -117,6 +123,1867 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kpl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-FCF9-4B24-A7E2-B8225492598B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-FCF9-4B24-A7E2-B8225492598B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="2E-3"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$M$35:$N$35</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Benign</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cancer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$36:$N$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.5166594846852408E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7560152507848932E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FCF9-4B24-A7E2-B8225492598B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="555498064"/>
+        <c:axId val="555492160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="555498064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555492160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="555492160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="555498064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>kLEfflux</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F16D-4E61-8BE1-15E1D75746CF}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$R$36:$S$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>6.7513944016994775E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.9487075975164306E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$R$36:$S$36</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>6.7513944016994775E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.9487075975164306E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$R$34:$S$34</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Benign</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Cancer</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$35:$S$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.1401487816941433E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9918370364512568E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F16D-4E61-8BE1-15E1D75746CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="622264784"/>
+        <c:axId val="622265440"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="622264784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="622265440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="622265440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="622264784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>118110</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9B7148E-3C0C-46D7-A713-B2D2F3BB65F1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5DCD987-6894-46C2-9E6C-2CF5522624FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -416,10 +2283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DEAA74-06B0-40CB-82E5-B093011EF887}">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34:S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1426,7 +3293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>1</v>
@@ -1451,8 +3318,14 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="R34" t="s">
+        <v>2</v>
+      </c>
+      <c r="S34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>0</v>
       </c>
@@ -1462,8 +3335,23 @@
       <c r="D35" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="M35" t="s">
+        <v>2</v>
+      </c>
+      <c r="N35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>10</v>
+      </c>
+      <c r="R35">
+        <v>1.1401487816941433E-2</v>
+      </c>
+      <c r="S35">
+        <v>3.9918370364512568E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>3</v>
       </c>
@@ -1479,8 +3367,23 @@
         <f>AVERAGE(1/A$13,1/A$15,1/A$16,1/A$17)</f>
         <v>49.247446349649827</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="L36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36">
+        <v>2.5166594846852408E-3</v>
+      </c>
+      <c r="N36">
+        <v>1.7560152507848932E-2</v>
+      </c>
+      <c r="R36">
+        <v>6.7513944016994775E-3</v>
+      </c>
+      <c r="S36">
+        <v>1.9487075975164306E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B37">
         <f>STDEV(1/A$2,1/A$6,1/A$7,1/A$10)/SQRT(COUNT(A$2,A$6,A$7,A$10))</f>
         <v>0.4816902742794637</v>
@@ -1493,8 +3396,14 @@
         <f>STDEV(1/A$13,1/A$15,1/A$16,1/A$17)/SQRT(COUNT(A$13,A$15,A$16,A$17))</f>
         <v>0.69592632575157565</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="M37">
+        <v>2.135639041107119E-3</v>
+      </c>
+      <c r="N37">
+        <v>6.1619295870294138E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +3414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>4</v>
       </c>
@@ -1522,7 +3431,7 @@
         <v>2.5166594846852408E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C40">
         <f>STDEV(B$2,B$6,B$7,B$10)/SQRT(COUNT(B$2,B$6,B$7,B$10))</f>
         <v>3.8126329142850256E-3</v>
@@ -1536,7 +3445,7 @@
         <v>2.135639041107119E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D41" t="s">
         <v>0</v>
       </c>
@@ -1547,7 +3456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>5</v>
       </c>
@@ -1564,7 +3473,7 @@
         <v>1.2622907122063194</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D43">
         <f>STDEV(C$2,C$6,C$7,C$10)/SQRT(COUNT(C$2,C$6,C$7,C$10))</f>
         <v>5.7996467137492642</v>
@@ -1578,7 +3487,7 @@
         <v>0.95935243719443841</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E44" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +3498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D45" t="s">
         <v>6</v>
       </c>
@@ -1606,7 +3515,7 @@
         <v>7.4328838587104269E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E46">
         <f>STDEV(D$2,D$6,D$7,D$10)/SQRT(COUNT(D$2,D$6,D$7,D$10))</f>
         <v>8.7671984902016275E-9</v>
@@ -1620,7 +3529,7 @@
         <v>6.6251381835706622E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
       <c r="F47" t="s">
         <v>0</v>
       </c>
@@ -1631,7 +3540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
       <c r="E48" t="s">
         <v>7</v>
       </c>
@@ -1742,5 +3651,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>